<commit_message>
Implement heap operations and update project files
Completed heapifyDown and improved heap methods in Heap.cpp, updated main.cpp to test heap insertion and removal, and enhanced Makefile with clean and zip targets. Removed debug output, added error handling for empty heap, and updated VSCode settings. Added A6_Report.docx and project zip, updated rubric, and removed build artifacts.
</commit_message>
<xml_diff>
--- a/A6 codebase/A6 Self-scoring Rubric.xlsx
+++ b/A6 codebase/A6 Self-scoring Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Office com backup\UCO lectures\C++\CMSC2613-Intermediate\Assignments\F2025 Assignments\A6 minHeap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrah\OneDrive\Documents\GitHub\Fundamental-Data-Structures\A6 codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E80FD6FD-E7C1-4410-91A0-B757694F3253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB3FF54-7889-42E6-8327-DE2C50C78755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{821355E3-60BE-4892-B1A3-B4E71FC82347}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{821355E3-60BE-4892-B1A3-B4E71FC82347}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
     <t>A6 Implementing a minHeap with Exception Handling</t>
   </si>
   <si>
-    <t>Name:</t>
+    <t>Name: Abraham Khan</t>
   </si>
 </sst>
 </file>
@@ -206,10 +206,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,18 +548,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F303C946-F569-4262-B586-1E59010AB7EC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -567,15 +567,15 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -599,9 +599,11 @@
       <c r="C4" s="1">
         <v>20</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -609,9 +611,11 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -619,9 +623,11 @@
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -631,9 +637,11 @@
       <c r="C7" s="1">
         <v>15</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -641,9 +649,11 @@
       <c r="C8" s="1">
         <v>10</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -651,9 +661,11 @@
       <c r="C9" s="1">
         <v>10</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -663,9 +675,11 @@
       <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -673,9 +687,11 @@
       <c r="C11" s="1">
         <v>6</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -683,9 +699,11 @@
       <c r="C12" s="1">
         <v>6</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -695,9 +713,11 @@
       <c r="C13" s="1">
         <v>10</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
@@ -708,7 +728,7 @@
       </c>
       <c r="D14" s="1">
         <f>SUM(D4:D13)</f>
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>